<commit_message>
cetak pdh susulan dp5t38 dp3n20 pdu taruna
</commit_message>
<xml_diff>
--- a/4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)/UKURANS.xlsx
+++ b/4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)/UKURANS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\4. PDH DP 3N30 (MERAH) 3T25(COKLAT MUDA) 4N31(PUTIH) 5N38(HIJAU TUA) 5T38(PINKMUDA)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1B3ACE-6835-4210-9603-AA90CF6D2980}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99341E1-123E-4473-B783-C0DFE8A74020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="127">
   <si>
     <t>NO</t>
   </si>
@@ -404,6 +404,9 @@
   <si>
     <t>WIDODO</t>
   </si>
+  <si>
+    <t>M. FARID SAMODRA</t>
+  </si>
 </sst>
 </file>
 
@@ -764,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU417"/>
+  <dimension ref="A1:AU418"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="N49" zoomScale="86" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AF87" sqref="AF87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9060,21 +9063,51 @@
       <c r="AU86" s="2"/>
     </row>
     <row r="87" spans="1:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
-      <c r="O87" s="1"/>
+      <c r="A87" s="2">
+        <v>20</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E87" s="1">
+        <v>42</v>
+      </c>
+      <c r="F87" s="1">
+        <v>55</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H87" s="1">
+        <v>46</v>
+      </c>
+      <c r="I87" s="1">
+        <v>23</v>
+      </c>
+      <c r="J87" s="1">
+        <v>17</v>
+      </c>
+      <c r="K87" s="1">
+        <v>26</v>
+      </c>
+      <c r="L87" s="1">
+        <v>25</v>
+      </c>
+      <c r="M87" s="1">
+        <v>26</v>
+      </c>
+      <c r="N87" s="1">
+        <v>66</v>
+      </c>
+      <c r="O87" s="1">
+        <v>38</v>
+      </c>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
@@ -9084,13 +9117,27 @@
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
-      <c r="Y87" s="1"/>
-      <c r="Z87" s="1"/>
-      <c r="AA87" s="1"/>
-      <c r="AB87" s="1"/>
-      <c r="AC87" s="1"/>
-      <c r="AD87" s="1"/>
-      <c r="AE87" s="1"/>
+      <c r="Y87" s="1">
+        <v>74</v>
+      </c>
+      <c r="Z87" s="1">
+        <v>90</v>
+      </c>
+      <c r="AA87" s="1">
+        <v>67</v>
+      </c>
+      <c r="AB87" s="1">
+        <v>29</v>
+      </c>
+      <c r="AC87" s="1">
+        <v>24</v>
+      </c>
+      <c r="AD87" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE87" s="1">
+        <v>97</v>
+      </c>
       <c r="AF87" s="2"/>
       <c r="AG87" s="2"/>
       <c r="AH87" s="2"/>
@@ -9109,12 +9156,8 @@
       <c r="AU87" s="2"/>
     </row>
     <row r="88" spans="1:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="2">
-        <v>20</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -9162,8 +9205,12 @@
       <c r="AU88" s="2"/>
     </row>
     <row r="89" spans="1:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
+      <c r="A89" s="2">
+        <v>20</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -10122,7 +10169,7 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
       <c r="AC108" s="1"/>
-      <c r="AD108" s="2"/>
+      <c r="AD108" s="1"/>
       <c r="AE108" s="1"/>
       <c r="AF108" s="2"/>
       <c r="AG108" s="2"/>
@@ -13994,7 +14041,7 @@
       <c r="AB187" s="1"/>
       <c r="AC187" s="1"/>
       <c r="AD187" s="2"/>
-      <c r="AE187" s="2"/>
+      <c r="AE187" s="1"/>
       <c r="AF187" s="2"/>
       <c r="AG187" s="2"/>
       <c r="AH187" s="2"/>
@@ -14505,33 +14552,33 @@
     <row r="198" spans="1:47" ht="15" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
-      <c r="D198" s="2"/>
-      <c r="E198" s="2"/>
-      <c r="F198" s="2"/>
-      <c r="G198" s="2"/>
-      <c r="H198" s="2"/>
-      <c r="I198" s="2"/>
-      <c r="J198" s="2"/>
-      <c r="K198" s="2"/>
-      <c r="L198" s="2"/>
-      <c r="M198" s="2"/>
-      <c r="N198" s="2"/>
-      <c r="O198" s="2"/>
-      <c r="P198" s="2"/>
-      <c r="Q198" s="2"/>
-      <c r="R198" s="2"/>
-      <c r="S198" s="2"/>
-      <c r="T198" s="2"/>
-      <c r="U198" s="2"/>
-      <c r="V198" s="2"/>
-      <c r="W198" s="2"/>
-      <c r="X198" s="2"/>
-      <c r="Y198" s="2"/>
-      <c r="Z198" s="2"/>
-      <c r="AA198" s="2"/>
-      <c r="AB198" s="2"/>
-      <c r="AC198" s="2"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="1"/>
+      <c r="F198" s="1"/>
+      <c r="G198" s="1"/>
+      <c r="H198" s="1"/>
+      <c r="I198" s="1"/>
+      <c r="J198" s="1"/>
+      <c r="K198" s="1"/>
+      <c r="L198" s="1"/>
+      <c r="M198" s="1"/>
+      <c r="N198" s="1"/>
+      <c r="O198" s="1"/>
+      <c r="P198" s="1"/>
+      <c r="Q198" s="1"/>
+      <c r="R198" s="1"/>
+      <c r="S198" s="1"/>
+      <c r="T198" s="1"/>
+      <c r="U198" s="1"/>
+      <c r="V198" s="1"/>
+      <c r="W198" s="1"/>
+      <c r="X198" s="1"/>
+      <c r="Y198" s="1"/>
+      <c r="Z198" s="1"/>
+      <c r="AA198" s="1"/>
+      <c r="AB198" s="1"/>
+      <c r="AC198" s="1"/>
       <c r="AD198" s="2"/>
       <c r="AE198" s="2"/>
       <c r="AF198" s="2"/>
@@ -25282,6 +25329,55 @@
       <c r="AT417" s="2"/>
       <c r="AU417" s="2"/>
     </row>
+    <row r="418" spans="1:47" ht="15" x14ac:dyDescent="0.2">
+      <c r="A418" s="2"/>
+      <c r="B418" s="2"/>
+      <c r="C418" s="2"/>
+      <c r="D418" s="2"/>
+      <c r="E418" s="2"/>
+      <c r="F418" s="2"/>
+      <c r="G418" s="2"/>
+      <c r="H418" s="2"/>
+      <c r="I418" s="2"/>
+      <c r="J418" s="2"/>
+      <c r="K418" s="2"/>
+      <c r="L418" s="2"/>
+      <c r="M418" s="2"/>
+      <c r="N418" s="2"/>
+      <c r="O418" s="2"/>
+      <c r="P418" s="2"/>
+      <c r="Q418" s="2"/>
+      <c r="R418" s="2"/>
+      <c r="S418" s="2"/>
+      <c r="T418" s="2"/>
+      <c r="U418" s="2"/>
+      <c r="V418" s="2"/>
+      <c r="W418" s="2"/>
+      <c r="X418" s="2"/>
+      <c r="Y418" s="2"/>
+      <c r="Z418" s="2"/>
+      <c r="AA418" s="2"/>
+      <c r="AB418" s="2"/>
+      <c r="AC418" s="2"/>
+      <c r="AD418" s="2"/>
+      <c r="AE418" s="2"/>
+      <c r="AF418" s="2"/>
+      <c r="AG418" s="2"/>
+      <c r="AH418" s="2"/>
+      <c r="AI418" s="2"/>
+      <c r="AJ418" s="2"/>
+      <c r="AK418" s="2"/>
+      <c r="AL418" s="2"/>
+      <c r="AM418" s="2"/>
+      <c r="AN418" s="2"/>
+      <c r="AO418" s="2"/>
+      <c r="AP418" s="2"/>
+      <c r="AQ418" s="2"/>
+      <c r="AR418" s="2"/>
+      <c r="AS418" s="2"/>
+      <c r="AT418" s="2"/>
+      <c r="AU418" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>